<commit_message>
merge du code des autres dans la version
</commit_message>
<xml_diff>
--- a/Documents/NetBeansProjects/TP1/configurationTests/Explication_Cas_DDC2.xlsx
+++ b/Documents/NetBeansProjects/TP1/configurationTests/Explication_Cas_DDC2.xlsx
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>